<commit_message>
add feature select all sheet, and combine all sheets, adn add bar chart as analysis
</commit_message>
<xml_diff>
--- a/dataset/template.xlsx
+++ b/dataset/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gamesh Arwan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gamesh Arwan\Downloads\SKRIPSI\Skripsi Streamlit\indonesia-province-ghg-cluster-map\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC11A7E-7076-4461-B39B-B7132B99D9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0502718-B58B-41EF-B4CA-6231AA12C4E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" tabRatio="959" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,9 +121,6 @@
     <t>Sumatera Utara</t>
   </si>
   <si>
-    <t>PROVINSI</t>
-  </si>
-  <si>
     <t>DI Yogyakarta</t>
   </si>
   <si>
@@ -233,6 +230,9 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>PROVINCE</t>
   </si>
 </sst>
 </file>
@@ -606,7 +606,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -617,10 +617,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="C1">
         <v>2000</v>
@@ -628,7 +628,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -636,7 +636,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -660,15 +660,15 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -676,7 +676,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -692,7 +692,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
@@ -708,7 +708,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -716,7 +716,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
@@ -724,7 +724,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
@@ -732,7 +732,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
@@ -740,7 +740,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
@@ -748,7 +748,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
         <v>19</v>
@@ -756,15 +756,15 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
@@ -772,7 +772,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
@@ -780,7 +780,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
@@ -788,7 +788,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
         <v>0</v>
@@ -796,7 +796,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
@@ -804,7 +804,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
         <v>2</v>
@@ -812,7 +812,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
@@ -820,7 +820,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
@@ -828,7 +828,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
         <v>23</v>
@@ -836,7 +836,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
         <v>24</v>
@@ -844,7 +844,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
         <v>25</v>
@@ -852,7 +852,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
         <v>26</v>
@@ -860,7 +860,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
         <v>27</v>
@@ -868,7 +868,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
         <v>28</v>
@@ -876,7 +876,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
         <v>29</v>
@@ -884,7 +884,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s">
         <v>30</v>
@@ -892,7 +892,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B35" t="s">
         <v>31</v>

</xml_diff>